<commit_message>
Se arregla el load del pickle, faltaba la variable que iba a recibir el objeto
</commit_message>
<xml_diff>
--- a/centroides.xlsx
+++ b/centroides.xlsx
@@ -485,31 +485,31 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="C2" t="n">
         <v>1</v>
       </c>
       <c r="D2" t="n">
-        <v>-0</v>
+        <v>1</v>
       </c>
       <c r="E2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="I2" t="n">
-        <v>0.5713</v>
+        <v>0.5604</v>
       </c>
       <c r="J2" t="n">
-        <v>45.1327</v>
+        <v>44.2716</v>
       </c>
     </row>
     <row r="3">
@@ -526,7 +526,7 @@
         <v>1</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="F3" t="n">
         <v>0</v>
@@ -549,31 +549,31 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="C4" t="n">
         <v>1</v>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>-0</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F4" t="n">
         <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="H4" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="I4" t="n">
-        <v>0.5604</v>
+        <v>0.5713</v>
       </c>
       <c r="J4" t="n">
-        <v>44.2716</v>
+        <v>45.1327</v>
       </c>
     </row>
     <row r="5">
@@ -599,7 +599,7 @@
         <v>-0</v>
       </c>
       <c r="H5" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="I5" t="n">
         <v>0.5537</v>
@@ -613,10 +613,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6" t="n">
-        <v>1</v>
+        <v>-0</v>
       </c>
       <c r="D6" t="n">
         <v>-0</v>
@@ -625,7 +625,7 @@
         <v>-0</v>
       </c>
       <c r="F6" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="G6" t="n">
         <v>-0</v>
@@ -634,10 +634,10 @@
         <v>1</v>
       </c>
       <c r="I6" t="n">
-        <v>0.5339</v>
+        <v>0.5661</v>
       </c>
       <c r="J6" t="n">
-        <v>42.1781</v>
+        <v>44.72190000000001</v>
       </c>
     </row>
     <row r="7">
@@ -645,10 +645,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7" t="n">
         <v>0</v>
@@ -666,10 +666,10 @@
         <v>1</v>
       </c>
       <c r="I7" t="n">
-        <v>0.5661</v>
+        <v>0.5339</v>
       </c>
       <c r="J7" t="n">
-        <v>44.72190000000001</v>
+        <v>42.1781</v>
       </c>
     </row>
     <row r="8">
@@ -677,10 +677,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8" t="n">
         <v>0</v>
@@ -689,19 +689,19 @@
         <v>-0</v>
       </c>
       <c r="F8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>-0</v>
+        <v>1</v>
       </c>
       <c r="H8" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="I8" t="n">
-        <v>0.5737</v>
+        <v>0.5513</v>
       </c>
       <c r="J8" t="n">
-        <v>45.3223</v>
+        <v>43.5527</v>
       </c>
     </row>
     <row r="9">
@@ -709,10 +709,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D9" t="n">
         <v>0</v>
@@ -730,10 +730,10 @@
         <v>-0</v>
       </c>
       <c r="I9" t="n">
-        <v>0.5513</v>
+        <v>0.5456</v>
       </c>
       <c r="J9" t="n">
-        <v>43.5527</v>
+        <v>43.1024</v>
       </c>
     </row>
     <row r="10">
@@ -753,19 +753,19 @@
         <v>-0</v>
       </c>
       <c r="F10" t="n">
-        <v>-0</v>
+        <v>1</v>
       </c>
       <c r="G10" t="n">
-        <v>1</v>
+        <v>-0</v>
       </c>
       <c r="H10" t="n">
         <v>-0</v>
       </c>
       <c r="I10" t="n">
-        <v>0.5456</v>
+        <v>0.5737</v>
       </c>
       <c r="J10" t="n">
-        <v>43.1024</v>
+        <v>45.3223</v>
       </c>
     </row>
     <row r="11">
@@ -788,7 +788,7 @@
         <v>1</v>
       </c>
       <c r="G11" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="H11" t="n">
         <v>-0</v>

</xml_diff>

<commit_message>
Se agrego un ejemplo de como predecir con el objeto modelo_kmeans
</commit_message>
<xml_diff>
--- a/centroides.xlsx
+++ b/centroides.xlsx
@@ -485,31 +485,31 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="C2" t="n">
         <v>1</v>
       </c>
       <c r="D2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G2" t="n">
         <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="I2" t="n">
-        <v>0.5604</v>
+        <v>0.5845</v>
       </c>
       <c r="J2" t="n">
-        <v>44.2716</v>
+        <v>46.1755</v>
       </c>
     </row>
     <row r="3">
@@ -549,31 +549,31 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="C4" t="n">
         <v>1</v>
       </c>
       <c r="D4" t="n">
-        <v>-0</v>
+        <v>1</v>
       </c>
       <c r="E4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4" t="n">
         <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="H4" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="I4" t="n">
-        <v>0.5713</v>
+        <v>0.5604</v>
       </c>
       <c r="J4" t="n">
-        <v>45.1327</v>
+        <v>44.2716</v>
       </c>
     </row>
     <row r="5">
@@ -581,31 +581,31 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5" t="n">
         <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>1</v>
+        <v>-0</v>
       </c>
       <c r="F5" t="n">
         <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>-0</v>
+        <v>1</v>
       </c>
       <c r="H5" t="n">
         <v>0</v>
       </c>
       <c r="I5" t="n">
-        <v>0.5537</v>
+        <v>0.5513</v>
       </c>
       <c r="J5" t="n">
-        <v>43.7423</v>
+        <v>43.5527</v>
       </c>
     </row>
     <row r="6">
@@ -613,16 +613,16 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>-0</v>
+        <v>1</v>
       </c>
       <c r="D6" t="n">
         <v>-0</v>
       </c>
       <c r="E6" t="n">
-        <v>-0</v>
+        <v>1</v>
       </c>
       <c r="F6" t="n">
         <v>0</v>
@@ -631,13 +631,13 @@
         <v>-0</v>
       </c>
       <c r="H6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I6" t="n">
-        <v>0.5661</v>
+        <v>0.5713</v>
       </c>
       <c r="J6" t="n">
-        <v>44.72190000000001</v>
+        <v>45.1327</v>
       </c>
     </row>
     <row r="7">
@@ -645,16 +645,16 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D7" t="n">
         <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>-0</v>
+        <v>1</v>
       </c>
       <c r="F7" t="n">
         <v>0</v>
@@ -663,13 +663,13 @@
         <v>-0</v>
       </c>
       <c r="H7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I7" t="n">
-        <v>0.5339</v>
+        <v>0.5537</v>
       </c>
       <c r="J7" t="n">
-        <v>42.1781</v>
+        <v>43.7423</v>
       </c>
     </row>
     <row r="8">
@@ -683,7 +683,7 @@
         <v>1</v>
       </c>
       <c r="D8" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="E8" t="n">
         <v>-0</v>
@@ -692,16 +692,16 @@
         <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>1</v>
+        <v>-0</v>
       </c>
       <c r="H8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I8" t="n">
-        <v>0.5513</v>
+        <v>0.5339</v>
       </c>
       <c r="J8" t="n">
-        <v>43.5527</v>
+        <v>42.1781</v>
       </c>
     </row>
     <row r="9">
@@ -712,10 +712,10 @@
         <v>1</v>
       </c>
       <c r="C9" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="D9" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="E9" t="n">
         <v>-0</v>
@@ -724,16 +724,16 @@
         <v>0</v>
       </c>
       <c r="G9" t="n">
-        <v>1</v>
+        <v>-0</v>
       </c>
       <c r="H9" t="n">
-        <v>-0</v>
+        <v>1</v>
       </c>
       <c r="I9" t="n">
-        <v>0.5456</v>
+        <v>0.5661</v>
       </c>
       <c r="J9" t="n">
-        <v>43.1024</v>
+        <v>44.72190000000001</v>
       </c>
     </row>
     <row r="10">
@@ -773,10 +773,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D11" t="n">
         <v>0</v>
@@ -785,19 +785,19 @@
         <v>-0</v>
       </c>
       <c r="F11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H11" t="n">
         <v>-0</v>
       </c>
       <c r="I11" t="n">
-        <v>0.5845</v>
+        <v>0.5456</v>
       </c>
       <c r="J11" t="n">
-        <v>46.1755</v>
+        <v>43.1024</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
se modifico los reshape y se cambio por doble corchete [[ ]]
</commit_message>
<xml_diff>
--- a/centroides.xlsx
+++ b/centroides.xlsx
@@ -485,31 +485,31 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="C2" t="n">
         <v>1</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G2" t="n">
         <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="I2" t="n">
-        <v>0.5845</v>
+        <v>0.5604</v>
       </c>
       <c r="J2" t="n">
-        <v>46.1755</v>
+        <v>44.2716</v>
       </c>
     </row>
     <row r="3">
@@ -549,31 +549,31 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="C4" t="n">
         <v>1</v>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="F4" t="n">
         <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H4" t="n">
         <v>-0</v>
       </c>
       <c r="I4" t="n">
-        <v>0.5604</v>
+        <v>0.5513</v>
       </c>
       <c r="J4" t="n">
-        <v>44.2716</v>
+        <v>43.5527</v>
       </c>
     </row>
     <row r="5">
@@ -581,10 +581,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5" t="n">
         <v>0</v>
@@ -596,16 +596,16 @@
         <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>1</v>
+        <v>-0</v>
       </c>
       <c r="H5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I5" t="n">
-        <v>0.5513</v>
+        <v>0.5661</v>
       </c>
       <c r="J5" t="n">
-        <v>43.5527</v>
+        <v>44.72190000000001</v>
       </c>
     </row>
     <row r="6">
@@ -619,7 +619,7 @@
         <v>1</v>
       </c>
       <c r="D6" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="E6" t="n">
         <v>1</v>
@@ -663,7 +663,7 @@
         <v>-0</v>
       </c>
       <c r="H7" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="I7" t="n">
         <v>0.5537</v>
@@ -689,7 +689,7 @@
         <v>-0</v>
       </c>
       <c r="F8" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="G8" t="n">
         <v>-0</v>
@@ -712,10 +712,10 @@
         <v>1</v>
       </c>
       <c r="C9" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="E9" t="n">
         <v>-0</v>
@@ -724,16 +724,16 @@
         <v>0</v>
       </c>
       <c r="G9" t="n">
-        <v>-0</v>
+        <v>1</v>
       </c>
       <c r="H9" t="n">
-        <v>1</v>
+        <v>-0</v>
       </c>
       <c r="I9" t="n">
-        <v>0.5661</v>
+        <v>0.5456</v>
       </c>
       <c r="J9" t="n">
-        <v>44.72190000000001</v>
+        <v>43.1024</v>
       </c>
     </row>
     <row r="10">
@@ -756,7 +756,7 @@
         <v>1</v>
       </c>
       <c r="G10" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="H10" t="n">
         <v>-0</v>
@@ -773,10 +773,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11" t="n">
         <v>0</v>
@@ -785,19 +785,19 @@
         <v>-0</v>
       </c>
       <c r="F11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H11" t="n">
         <v>-0</v>
       </c>
       <c r="I11" t="n">
-        <v>0.5456</v>
+        <v>0.5845</v>
       </c>
       <c r="J11" t="n">
-        <v>43.1024</v>
+        <v>46.1755</v>
       </c>
     </row>
   </sheetData>

</xml_diff>